<commit_message>
fixed child_id + row_id columns in dictionaires
</commit_message>
<xml_diff>
--- a/dictionaries/chemicals_ath/1_0/1_0_yearly_rep.xlsx
+++ b/dictionaries/chemicals_ath/1_0/1_0_yearly_rep.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\alldicts\12jul2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\20220613_dicts\alldicts\14jul2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084D04A7-0DDB-4354-8C85-86CB2DAF5C96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161BDD76-DE51-4E84-9921-99A3D4B0C008}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="180">
   <si>
     <t>table</t>
   </si>
@@ -43,539 +43,536 @@
     <t>label</t>
   </si>
   <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>child_id</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Unique identifer for the child</t>
+  </si>
+  <si>
+    <t>age_years</t>
+  </si>
+  <si>
+    <t>Age of child in years</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>label:en</t>
+  </si>
+  <si>
+    <t>c_bps_raw_</t>
+  </si>
+  <si>
+    <t>µg/L</t>
+  </si>
+  <si>
+    <t>child urine BPS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_bps_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine BPS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c_bpf_raw_ </t>
+  </si>
+  <si>
+    <t>Child urine BPF levels at # years</t>
+  </si>
+  <si>
+    <t>c_bpf_lod_</t>
+  </si>
+  <si>
+    <t>Limit of detection of child urine BPF at # years</t>
+  </si>
+  <si>
+    <t>c_etpa_raw_</t>
+  </si>
+  <si>
+    <t>child urine ETPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_etpa_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine ETPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_trcs_raw_</t>
+  </si>
+  <si>
+    <t>child urine TRCS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_trcs_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine TRCS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mibp_raw_</t>
+  </si>
+  <si>
+    <t>child urine MiBP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mibp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MiBP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mbzp_raw_</t>
+  </si>
+  <si>
+    <t>child urine MBzP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mbzp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MBzP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mehhp_raw_</t>
+  </si>
+  <si>
+    <t>child urine MEHHP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mehhp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MEHHP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mecpp_raw_</t>
+  </si>
+  <si>
+    <t>child urine MECPP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mecpp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MECPP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_ohminp_raw_</t>
+  </si>
+  <si>
+    <t>child urine ohminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_ohminp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine ohminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cxminp_raw_</t>
+  </si>
+  <si>
+    <t>child urine cxminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cxminp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine cxminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_ohminch_raw_</t>
+  </si>
+  <si>
+    <t>child urine ohminch levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_ohminch_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine ohminch levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mnpep_raw_</t>
+  </si>
+  <si>
+    <t>child urine MnPeP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mnpep_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MnPeP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mnop_raw_</t>
+  </si>
+  <si>
+    <t>child urine MnOP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mnop_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MnOP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mhxp_raw_</t>
+  </si>
+  <si>
+    <t>child urine mHxP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_mhxp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine mHxP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pfhps_raw_</t>
+  </si>
+  <si>
+    <t>child PFHpS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pfhps_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child PFHpS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pfoa_raw_</t>
+  </si>
+  <si>
+    <t>child PFOA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pfoa_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child PFOA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pfda_raw_</t>
+  </si>
+  <si>
+    <t>child PFDA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pfda_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child PFDA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pcb138_raw_</t>
+  </si>
+  <si>
+    <t>pg/g</t>
+  </si>
+  <si>
+    <t>child PCB-138 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pcb138_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child PCB-138 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pcb170_raw_</t>
+  </si>
+  <si>
+    <t>child PCB-170 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pcb170_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child PCB-170 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_ddt_raw_</t>
+  </si>
+  <si>
+    <t>child DDT levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_ddt_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child DDT levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_hcb_raw_</t>
+  </si>
+  <si>
+    <t>child HCB levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_hcb_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child HCB levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pbde47_raw_</t>
+  </si>
+  <si>
+    <t>child PBDE-47 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pbde47_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child PBDE-47 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cd_raw_</t>
+  </si>
+  <si>
+    <t>child Cd levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cd_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child Cd levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_se_raw_</t>
+  </si>
+  <si>
+    <t>child Se levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_se_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child Se levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_zn_raw_</t>
+  </si>
+  <si>
+    <t>child Zn levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_zn_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child Zn levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_tl_raw_</t>
+  </si>
+  <si>
+    <t>child Tl levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_tl_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child Tl levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cu_raw_</t>
+  </si>
+  <si>
+    <t>child Cu levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cu_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child Cu levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cs_raw_</t>
+  </si>
+  <si>
+    <t>child Cs levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_cs_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child Cs levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_k_raw_</t>
+  </si>
+  <si>
+    <t>child K levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_k_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child K levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_dmtp_raw_</t>
+  </si>
+  <si>
+    <t>child urine DMTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_dmtp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine DMTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_dep_raw_</t>
+  </si>
+  <si>
+    <t>child urine DEP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_dep_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine DEP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_dedtp_raw_</t>
+  </si>
+  <si>
+    <t>child urine DEDTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_dedtp_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine DEDTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_chrsene_raw_</t>
+  </si>
+  <si>
+    <t>child urine chrysene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_chrsene_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine chrysene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_napthalene_raw_</t>
+  </si>
+  <si>
+    <t>child urine Napthalene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_napthalene_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine Napthalene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_prene_raw_</t>
+  </si>
+  <si>
+    <t>child urine Pyrene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_prene_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine Pyrene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pyrethroids_raw_</t>
+  </si>
+  <si>
+    <t>child urine Pyrethroids levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_pyrethroids_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine Pyrethroids levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_imazalil_raw_</t>
+  </si>
+  <si>
+    <t>child urine Imazalil levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_imazalil_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine Imazalil levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_maa_raw_</t>
+  </si>
+  <si>
+    <t>child urine MAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_maa_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine MAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_eaa_raw_</t>
+  </si>
+  <si>
+    <t>child urine EAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_eaa_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine EAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_2mpa_raw_</t>
+  </si>
+  <si>
+    <t>child urine 2-MPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>c_2mpa_lod_</t>
+  </si>
+  <si>
+    <t>limit of detection of child urine 2-MPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
     <t>row_id</t>
   </si>
   <si>
-    <t>integer</t>
+    <t>numeric</t>
   </si>
   <si>
     <t>Unique identifer for the row in Opal</t>
-  </si>
-  <si>
-    <t>child_id</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Unique identifer for the child</t>
-  </si>
-  <si>
-    <t>cohort</t>
-  </si>
-  <si>
-    <t>Cohort</t>
-  </si>
-  <si>
-    <t>age_years</t>
-  </si>
-  <si>
-    <t>Age of child in years</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>label:en</t>
-  </si>
-  <si>
-    <t>c_bps_raw_</t>
-  </si>
-  <si>
-    <t>µg/L</t>
-  </si>
-  <si>
-    <t>child urine BPS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_bps_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine BPS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c_bpf_raw_ </t>
-  </si>
-  <si>
-    <t>Child urine BPF levels at # years</t>
-  </si>
-  <si>
-    <t>c_bpf_lod_</t>
-  </si>
-  <si>
-    <t>Limit of detection of child urine BPF at # years</t>
-  </si>
-  <si>
-    <t>c_etpa_raw_</t>
-  </si>
-  <si>
-    <t>child urine ETPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_etpa_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine ETPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_trcs_raw_</t>
-  </si>
-  <si>
-    <t>child urine TRCS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_trcs_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine TRCS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mibp_raw_</t>
-  </si>
-  <si>
-    <t>child urine MiBP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mibp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MiBP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mbzp_raw_</t>
-  </si>
-  <si>
-    <t>child urine MBzP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mbzp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MBzP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mehhp_raw_</t>
-  </si>
-  <si>
-    <t>child urine MEHHP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mehhp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MEHHP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mecpp_raw_</t>
-  </si>
-  <si>
-    <t>child urine MECPP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mecpp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MECPP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_ohminp_raw_</t>
-  </si>
-  <si>
-    <t>child urine ohminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_ohminp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine ohminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cxminp_raw_</t>
-  </si>
-  <si>
-    <t>child urine cxminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cxminp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine cxminp levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_ohminch_raw_</t>
-  </si>
-  <si>
-    <t>child urine ohminch levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_ohminch_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine ohminch levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mnpep_raw_</t>
-  </si>
-  <si>
-    <t>child urine MnPeP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mnpep_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MnPeP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mnop_raw_</t>
-  </si>
-  <si>
-    <t>child urine MnOP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mnop_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MnOP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mhxp_raw_</t>
-  </si>
-  <si>
-    <t>child urine mHxP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_mhxp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine mHxP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pfhps_raw_</t>
-  </si>
-  <si>
-    <t>child PFHpS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pfhps_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child PFHpS levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pfoa_raw_</t>
-  </si>
-  <si>
-    <t>child PFOA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pfoa_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child PFOA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pfda_raw_</t>
-  </si>
-  <si>
-    <t>child PFDA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pfda_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child PFDA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pcb138_raw_</t>
-  </si>
-  <si>
-    <t>pg/g</t>
-  </si>
-  <si>
-    <t>child PCB-138 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pcb138_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child PCB-138 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pcb170_raw_</t>
-  </si>
-  <si>
-    <t>child PCB-170 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pcb170_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child PCB-170 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_ddt_raw_</t>
-  </si>
-  <si>
-    <t>child DDT levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_ddt_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child DDT levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_hcb_raw_</t>
-  </si>
-  <si>
-    <t>child HCB levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_hcb_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child HCB levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pbde47_raw_</t>
-  </si>
-  <si>
-    <t>child PBDE-47 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pbde47_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child PBDE-47 levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cd_raw_</t>
-  </si>
-  <si>
-    <t>child Cd levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cd_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child Cd levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_se_raw_</t>
-  </si>
-  <si>
-    <t>child Se levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_se_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child Se levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_zn_raw_</t>
-  </si>
-  <si>
-    <t>child Zn levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_zn_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child Zn levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_tl_raw_</t>
-  </si>
-  <si>
-    <t>child Tl levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_tl_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child Tl levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cu_raw_</t>
-  </si>
-  <si>
-    <t>child Cu levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cu_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child Cu levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cs_raw_</t>
-  </si>
-  <si>
-    <t>child Cs levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_cs_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child Cs levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_k_raw_</t>
-  </si>
-  <si>
-    <t>child K levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_k_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child K levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_dmtp_raw_</t>
-  </si>
-  <si>
-    <t>child urine DMTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_dmtp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine DMTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_dep_raw_</t>
-  </si>
-  <si>
-    <t>child urine DEP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_dep_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine DEP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_dedtp_raw_</t>
-  </si>
-  <si>
-    <t>child urine DEDTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_dedtp_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine DEDTP levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_chrsene_raw_</t>
-  </si>
-  <si>
-    <t>child urine chrysene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_chrsene_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine chrysene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_napthalene_raw_</t>
-  </si>
-  <si>
-    <t>child urine Napthalene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_napthalene_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine Napthalene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_prene_raw_</t>
-  </si>
-  <si>
-    <t>child urine Pyrene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_prene_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine Pyrene levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pyrethroids_raw_</t>
-  </si>
-  <si>
-    <t>child urine Pyrethroids levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_pyrethroids_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine Pyrethroids levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_imazalil_raw_</t>
-  </si>
-  <si>
-    <t>child urine Imazalil levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_imazalil_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine Imazalil levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_maa_raw_</t>
-  </si>
-  <si>
-    <t>child urine MAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_maa_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine MAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_eaa_raw_</t>
-  </si>
-  <si>
-    <t>child urine EAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_eaa_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine EAA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_2mpa_raw_</t>
-  </si>
-  <si>
-    <t>child urine 2-MPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>c_2mpa_lod_</t>
-  </si>
-  <si>
-    <t>limit of detection of child urine 2-MPA levels within # year of age (child was aged between # and &lt; #+1 year)</t>
-  </si>
-  <si>
-    <t>decimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -708,8 +705,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -822,6 +824,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -978,7 +986,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1001,6 +1009,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="20% - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1422,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMH176"/>
+  <dimension ref="A1:AMH175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1444,7 @@
     <col min="5" max="1022" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1022" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1449,1173 +1458,2184 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:1022" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
+      <c r="BI2"/>
+      <c r="BJ2"/>
+      <c r="BK2"/>
+      <c r="BL2"/>
+      <c r="BM2"/>
+      <c r="BN2"/>
+      <c r="BO2"/>
+      <c r="BP2"/>
+      <c r="BQ2"/>
+      <c r="BR2"/>
+      <c r="BS2"/>
+      <c r="BT2"/>
+      <c r="BU2"/>
+      <c r="BV2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+      <c r="CL2"/>
+      <c r="CM2"/>
+      <c r="CN2"/>
+      <c r="CO2"/>
+      <c r="CP2"/>
+      <c r="CQ2"/>
+      <c r="CR2"/>
+      <c r="CS2"/>
+      <c r="CT2"/>
+      <c r="CU2"/>
+      <c r="CV2"/>
+      <c r="CW2"/>
+      <c r="CX2"/>
+      <c r="CY2"/>
+      <c r="CZ2"/>
+      <c r="DA2"/>
+      <c r="DB2"/>
+      <c r="DC2"/>
+      <c r="DD2"/>
+      <c r="DE2"/>
+      <c r="DF2"/>
+      <c r="DG2"/>
+      <c r="DH2"/>
+      <c r="DI2"/>
+      <c r="DJ2"/>
+      <c r="DK2"/>
+      <c r="DL2"/>
+      <c r="DM2"/>
+      <c r="DN2"/>
+      <c r="DO2"/>
+      <c r="DP2"/>
+      <c r="DQ2"/>
+      <c r="DR2"/>
+      <c r="DS2"/>
+      <c r="DT2"/>
+      <c r="DU2"/>
+      <c r="DV2"/>
+      <c r="DW2"/>
+      <c r="DX2"/>
+      <c r="DY2"/>
+      <c r="DZ2"/>
+      <c r="EA2"/>
+      <c r="EB2"/>
+      <c r="EC2"/>
+      <c r="ED2"/>
+      <c r="EE2"/>
+      <c r="EF2"/>
+      <c r="EG2"/>
+      <c r="EH2"/>
+      <c r="EI2"/>
+      <c r="EJ2"/>
+      <c r="EK2"/>
+      <c r="EL2"/>
+      <c r="EM2"/>
+      <c r="EN2"/>
+      <c r="EO2"/>
+      <c r="EP2"/>
+      <c r="EQ2"/>
+      <c r="ER2"/>
+      <c r="ES2"/>
+      <c r="ET2"/>
+      <c r="EU2"/>
+      <c r="EV2"/>
+      <c r="EW2"/>
+      <c r="EX2"/>
+      <c r="EY2"/>
+      <c r="EZ2"/>
+      <c r="FA2"/>
+      <c r="FB2"/>
+      <c r="FC2"/>
+      <c r="FD2"/>
+      <c r="FE2"/>
+      <c r="FF2"/>
+      <c r="FG2"/>
+      <c r="FH2"/>
+      <c r="FI2"/>
+      <c r="FJ2"/>
+      <c r="FK2"/>
+      <c r="FL2"/>
+      <c r="FM2"/>
+      <c r="FN2"/>
+      <c r="FO2"/>
+      <c r="FP2"/>
+      <c r="FQ2"/>
+      <c r="FR2"/>
+      <c r="FS2"/>
+      <c r="FT2"/>
+      <c r="FU2"/>
+      <c r="FV2"/>
+      <c r="FW2"/>
+      <c r="FX2"/>
+      <c r="FY2"/>
+      <c r="FZ2"/>
+      <c r="GA2"/>
+      <c r="GB2"/>
+      <c r="GC2"/>
+      <c r="GD2"/>
+      <c r="GE2"/>
+      <c r="GF2"/>
+      <c r="GG2"/>
+      <c r="GH2"/>
+      <c r="GI2"/>
+      <c r="GJ2"/>
+      <c r="GK2"/>
+      <c r="GL2"/>
+      <c r="GM2"/>
+      <c r="GN2"/>
+      <c r="GO2"/>
+      <c r="GP2"/>
+      <c r="GQ2"/>
+      <c r="GR2"/>
+      <c r="GS2"/>
+      <c r="GT2"/>
+      <c r="GU2"/>
+      <c r="GV2"/>
+      <c r="GW2"/>
+      <c r="GX2"/>
+      <c r="GY2"/>
+      <c r="GZ2"/>
+      <c r="HA2"/>
+      <c r="HB2"/>
+      <c r="HC2"/>
+      <c r="HD2"/>
+      <c r="HE2"/>
+      <c r="HF2"/>
+      <c r="HG2"/>
+      <c r="HH2"/>
+      <c r="HI2"/>
+      <c r="HJ2"/>
+      <c r="HK2"/>
+      <c r="HL2"/>
+      <c r="HM2"/>
+      <c r="HN2"/>
+      <c r="HO2"/>
+      <c r="HP2"/>
+      <c r="HQ2"/>
+      <c r="HR2"/>
+      <c r="HS2"/>
+      <c r="HT2"/>
+      <c r="HU2"/>
+      <c r="HV2"/>
+      <c r="HW2"/>
+      <c r="HX2"/>
+      <c r="HY2"/>
+      <c r="HZ2"/>
+      <c r="IA2"/>
+      <c r="IB2"/>
+      <c r="IC2"/>
+      <c r="ID2"/>
+      <c r="IE2"/>
+      <c r="IF2"/>
+      <c r="IG2"/>
+      <c r="IH2"/>
+      <c r="II2"/>
+      <c r="IJ2"/>
+      <c r="IK2"/>
+      <c r="IL2"/>
+      <c r="IM2"/>
+      <c r="IN2"/>
+      <c r="IO2"/>
+      <c r="IP2"/>
+      <c r="IQ2"/>
+      <c r="IR2"/>
+      <c r="IS2"/>
+      <c r="IT2"/>
+      <c r="IU2"/>
+      <c r="IV2"/>
+      <c r="IW2"/>
+      <c r="IX2"/>
+      <c r="IY2"/>
+      <c r="IZ2"/>
+      <c r="JA2"/>
+      <c r="JB2"/>
+      <c r="JC2"/>
+      <c r="JD2"/>
+      <c r="JE2"/>
+      <c r="JF2"/>
+      <c r="JG2"/>
+      <c r="JH2"/>
+      <c r="JI2"/>
+      <c r="JJ2"/>
+      <c r="JK2"/>
+      <c r="JL2"/>
+      <c r="JM2"/>
+      <c r="JN2"/>
+      <c r="JO2"/>
+      <c r="JP2"/>
+      <c r="JQ2"/>
+      <c r="JR2"/>
+      <c r="JS2"/>
+      <c r="JT2"/>
+      <c r="JU2"/>
+      <c r="JV2"/>
+      <c r="JW2"/>
+      <c r="JX2"/>
+      <c r="JY2"/>
+      <c r="JZ2"/>
+      <c r="KA2"/>
+      <c r="KB2"/>
+      <c r="KC2"/>
+      <c r="KD2"/>
+      <c r="KE2"/>
+      <c r="KF2"/>
+      <c r="KG2"/>
+      <c r="KH2"/>
+      <c r="KI2"/>
+      <c r="KJ2"/>
+      <c r="KK2"/>
+      <c r="KL2"/>
+      <c r="KM2"/>
+      <c r="KN2"/>
+      <c r="KO2"/>
+      <c r="KP2"/>
+      <c r="KQ2"/>
+      <c r="KR2"/>
+      <c r="KS2"/>
+      <c r="KT2"/>
+      <c r="KU2"/>
+      <c r="KV2"/>
+      <c r="KW2"/>
+      <c r="KX2"/>
+      <c r="KY2"/>
+      <c r="KZ2"/>
+      <c r="LA2"/>
+      <c r="LB2"/>
+      <c r="LC2"/>
+      <c r="LD2"/>
+      <c r="LE2"/>
+      <c r="LF2"/>
+      <c r="LG2"/>
+      <c r="LH2"/>
+      <c r="LI2"/>
+      <c r="LJ2"/>
+      <c r="LK2"/>
+      <c r="LL2"/>
+      <c r="LM2"/>
+      <c r="LN2"/>
+      <c r="LO2"/>
+      <c r="LP2"/>
+      <c r="LQ2"/>
+      <c r="LR2"/>
+      <c r="LS2"/>
+      <c r="LT2"/>
+      <c r="LU2"/>
+      <c r="LV2"/>
+      <c r="LW2"/>
+      <c r="LX2"/>
+      <c r="LY2"/>
+      <c r="LZ2"/>
+      <c r="MA2"/>
+      <c r="MB2"/>
+      <c r="MC2"/>
+      <c r="MD2"/>
+      <c r="ME2"/>
+      <c r="MF2"/>
+      <c r="MG2"/>
+      <c r="MH2"/>
+      <c r="MI2"/>
+      <c r="MJ2"/>
+      <c r="MK2"/>
+      <c r="ML2"/>
+      <c r="MM2"/>
+      <c r="MN2"/>
+      <c r="MO2"/>
+      <c r="MP2"/>
+      <c r="MQ2"/>
+      <c r="MR2"/>
+      <c r="MS2"/>
+      <c r="MT2"/>
+      <c r="MU2"/>
+      <c r="MV2"/>
+      <c r="MW2"/>
+      <c r="MX2"/>
+      <c r="MY2"/>
+      <c r="MZ2"/>
+      <c r="NA2"/>
+      <c r="NB2"/>
+      <c r="NC2"/>
+      <c r="ND2"/>
+      <c r="NE2"/>
+      <c r="NF2"/>
+      <c r="NG2"/>
+      <c r="NH2"/>
+      <c r="NI2"/>
+      <c r="NJ2"/>
+      <c r="NK2"/>
+      <c r="NL2"/>
+      <c r="NM2"/>
+      <c r="NN2"/>
+      <c r="NO2"/>
+      <c r="NP2"/>
+      <c r="NQ2"/>
+      <c r="NR2"/>
+      <c r="NS2"/>
+      <c r="NT2"/>
+      <c r="NU2"/>
+      <c r="NV2"/>
+      <c r="NW2"/>
+      <c r="NX2"/>
+      <c r="NY2"/>
+      <c r="NZ2"/>
+      <c r="OA2"/>
+      <c r="OB2"/>
+      <c r="OC2"/>
+      <c r="OD2"/>
+      <c r="OE2"/>
+      <c r="OF2"/>
+      <c r="OG2"/>
+      <c r="OH2"/>
+      <c r="OI2"/>
+      <c r="OJ2"/>
+      <c r="OK2"/>
+      <c r="OL2"/>
+      <c r="OM2"/>
+      <c r="ON2"/>
+      <c r="OO2"/>
+      <c r="OP2"/>
+      <c r="OQ2"/>
+      <c r="OR2"/>
+      <c r="OS2"/>
+      <c r="OT2"/>
+      <c r="OU2"/>
+      <c r="OV2"/>
+      <c r="OW2"/>
+      <c r="OX2"/>
+      <c r="OY2"/>
+      <c r="OZ2"/>
+      <c r="PA2"/>
+      <c r="PB2"/>
+      <c r="PC2"/>
+      <c r="PD2"/>
+      <c r="PE2"/>
+      <c r="PF2"/>
+      <c r="PG2"/>
+      <c r="PH2"/>
+      <c r="PI2"/>
+      <c r="PJ2"/>
+      <c r="PK2"/>
+      <c r="PL2"/>
+      <c r="PM2"/>
+      <c r="PN2"/>
+      <c r="PO2"/>
+      <c r="PP2"/>
+      <c r="PQ2"/>
+      <c r="PR2"/>
+      <c r="PS2"/>
+      <c r="PT2"/>
+      <c r="PU2"/>
+      <c r="PV2"/>
+      <c r="PW2"/>
+      <c r="PX2"/>
+      <c r="PY2"/>
+      <c r="PZ2"/>
+      <c r="QA2"/>
+      <c r="QB2"/>
+      <c r="QC2"/>
+      <c r="QD2"/>
+      <c r="QE2"/>
+      <c r="QF2"/>
+      <c r="QG2"/>
+      <c r="QH2"/>
+      <c r="QI2"/>
+      <c r="QJ2"/>
+      <c r="QK2"/>
+      <c r="QL2"/>
+      <c r="QM2"/>
+      <c r="QN2"/>
+      <c r="QO2"/>
+      <c r="QP2"/>
+      <c r="QQ2"/>
+      <c r="QR2"/>
+      <c r="QS2"/>
+      <c r="QT2"/>
+      <c r="QU2"/>
+      <c r="QV2"/>
+      <c r="QW2"/>
+      <c r="QX2"/>
+      <c r="QY2"/>
+      <c r="QZ2"/>
+      <c r="RA2"/>
+      <c r="RB2"/>
+      <c r="RC2"/>
+      <c r="RD2"/>
+      <c r="RE2"/>
+      <c r="RF2"/>
+      <c r="RG2"/>
+      <c r="RH2"/>
+      <c r="RI2"/>
+      <c r="RJ2"/>
+      <c r="RK2"/>
+      <c r="RL2"/>
+      <c r="RM2"/>
+      <c r="RN2"/>
+      <c r="RO2"/>
+      <c r="RP2"/>
+      <c r="RQ2"/>
+      <c r="RR2"/>
+      <c r="RS2"/>
+      <c r="RT2"/>
+      <c r="RU2"/>
+      <c r="RV2"/>
+      <c r="RW2"/>
+      <c r="RX2"/>
+      <c r="RY2"/>
+      <c r="RZ2"/>
+      <c r="SA2"/>
+      <c r="SB2"/>
+      <c r="SC2"/>
+      <c r="SD2"/>
+      <c r="SE2"/>
+      <c r="SF2"/>
+      <c r="SG2"/>
+      <c r="SH2"/>
+      <c r="SI2"/>
+      <c r="SJ2"/>
+      <c r="SK2"/>
+      <c r="SL2"/>
+      <c r="SM2"/>
+      <c r="SN2"/>
+      <c r="SO2"/>
+      <c r="SP2"/>
+      <c r="SQ2"/>
+      <c r="SR2"/>
+      <c r="SS2"/>
+      <c r="ST2"/>
+      <c r="SU2"/>
+      <c r="SV2"/>
+      <c r="SW2"/>
+      <c r="SX2"/>
+      <c r="SY2"/>
+      <c r="SZ2"/>
+      <c r="TA2"/>
+      <c r="TB2"/>
+      <c r="TC2"/>
+      <c r="TD2"/>
+      <c r="TE2"/>
+      <c r="TF2"/>
+      <c r="TG2"/>
+      <c r="TH2"/>
+      <c r="TI2"/>
+      <c r="TJ2"/>
+      <c r="TK2"/>
+      <c r="TL2"/>
+      <c r="TM2"/>
+      <c r="TN2"/>
+      <c r="TO2"/>
+      <c r="TP2"/>
+      <c r="TQ2"/>
+      <c r="TR2"/>
+      <c r="TS2"/>
+      <c r="TT2"/>
+      <c r="TU2"/>
+      <c r="TV2"/>
+      <c r="TW2"/>
+      <c r="TX2"/>
+      <c r="TY2"/>
+      <c r="TZ2"/>
+      <c r="UA2"/>
+      <c r="UB2"/>
+      <c r="UC2"/>
+      <c r="UD2"/>
+      <c r="UE2"/>
+      <c r="UF2"/>
+      <c r="UG2"/>
+      <c r="UH2"/>
+      <c r="UI2"/>
+      <c r="UJ2"/>
+      <c r="UK2"/>
+      <c r="UL2"/>
+      <c r="UM2"/>
+      <c r="UN2"/>
+      <c r="UO2"/>
+      <c r="UP2"/>
+      <c r="UQ2"/>
+      <c r="UR2"/>
+      <c r="US2"/>
+      <c r="UT2"/>
+      <c r="UU2"/>
+      <c r="UV2"/>
+      <c r="UW2"/>
+      <c r="UX2"/>
+      <c r="UY2"/>
+      <c r="UZ2"/>
+      <c r="VA2"/>
+      <c r="VB2"/>
+      <c r="VC2"/>
+      <c r="VD2"/>
+      <c r="VE2"/>
+      <c r="VF2"/>
+      <c r="VG2"/>
+      <c r="VH2"/>
+      <c r="VI2"/>
+      <c r="VJ2"/>
+      <c r="VK2"/>
+      <c r="VL2"/>
+      <c r="VM2"/>
+      <c r="VN2"/>
+      <c r="VO2"/>
+      <c r="VP2"/>
+      <c r="VQ2"/>
+      <c r="VR2"/>
+      <c r="VS2"/>
+      <c r="VT2"/>
+      <c r="VU2"/>
+      <c r="VV2"/>
+      <c r="VW2"/>
+      <c r="VX2"/>
+      <c r="VY2"/>
+      <c r="VZ2"/>
+      <c r="WA2"/>
+      <c r="WB2"/>
+      <c r="WC2"/>
+      <c r="WD2"/>
+      <c r="WE2"/>
+      <c r="WF2"/>
+      <c r="WG2"/>
+      <c r="WH2"/>
+      <c r="WI2"/>
+      <c r="WJ2"/>
+      <c r="WK2"/>
+      <c r="WL2"/>
+      <c r="WM2"/>
+      <c r="WN2"/>
+      <c r="WO2"/>
+      <c r="WP2"/>
+      <c r="WQ2"/>
+      <c r="WR2"/>
+      <c r="WS2"/>
+      <c r="WT2"/>
+      <c r="WU2"/>
+      <c r="WV2"/>
+      <c r="WW2"/>
+      <c r="WX2"/>
+      <c r="WY2"/>
+      <c r="WZ2"/>
+      <c r="XA2"/>
+      <c r="XB2"/>
+      <c r="XC2"/>
+      <c r="XD2"/>
+      <c r="XE2"/>
+      <c r="XF2"/>
+      <c r="XG2"/>
+      <c r="XH2"/>
+      <c r="XI2"/>
+      <c r="XJ2"/>
+      <c r="XK2"/>
+      <c r="XL2"/>
+      <c r="XM2"/>
+      <c r="XN2"/>
+      <c r="XO2"/>
+      <c r="XP2"/>
+      <c r="XQ2"/>
+      <c r="XR2"/>
+      <c r="XS2"/>
+      <c r="XT2"/>
+      <c r="XU2"/>
+      <c r="XV2"/>
+      <c r="XW2"/>
+      <c r="XX2"/>
+      <c r="XY2"/>
+      <c r="XZ2"/>
+      <c r="YA2"/>
+      <c r="YB2"/>
+      <c r="YC2"/>
+      <c r="YD2"/>
+      <c r="YE2"/>
+      <c r="YF2"/>
+      <c r="YG2"/>
+      <c r="YH2"/>
+      <c r="YI2"/>
+      <c r="YJ2"/>
+      <c r="YK2"/>
+      <c r="YL2"/>
+      <c r="YM2"/>
+      <c r="YN2"/>
+      <c r="YO2"/>
+      <c r="YP2"/>
+      <c r="YQ2"/>
+      <c r="YR2"/>
+      <c r="YS2"/>
+      <c r="YT2"/>
+      <c r="YU2"/>
+      <c r="YV2"/>
+      <c r="YW2"/>
+      <c r="YX2"/>
+      <c r="YY2"/>
+      <c r="YZ2"/>
+      <c r="ZA2"/>
+      <c r="ZB2"/>
+      <c r="ZC2"/>
+      <c r="ZD2"/>
+      <c r="ZE2"/>
+      <c r="ZF2"/>
+      <c r="ZG2"/>
+      <c r="ZH2"/>
+      <c r="ZI2"/>
+      <c r="ZJ2"/>
+      <c r="ZK2"/>
+      <c r="ZL2"/>
+      <c r="ZM2"/>
+      <c r="ZN2"/>
+      <c r="ZO2"/>
+      <c r="ZP2"/>
+      <c r="ZQ2"/>
+      <c r="ZR2"/>
+      <c r="ZS2"/>
+      <c r="ZT2"/>
+      <c r="ZU2"/>
+      <c r="ZV2"/>
+      <c r="ZW2"/>
+      <c r="ZX2"/>
+      <c r="ZY2"/>
+      <c r="ZZ2"/>
+      <c r="AAA2"/>
+      <c r="AAB2"/>
+      <c r="AAC2"/>
+      <c r="AAD2"/>
+      <c r="AAE2"/>
+      <c r="AAF2"/>
+      <c r="AAG2"/>
+      <c r="AAH2"/>
+      <c r="AAI2"/>
+      <c r="AAJ2"/>
+      <c r="AAK2"/>
+      <c r="AAL2"/>
+      <c r="AAM2"/>
+      <c r="AAN2"/>
+      <c r="AAO2"/>
+      <c r="AAP2"/>
+      <c r="AAQ2"/>
+      <c r="AAR2"/>
+      <c r="AAS2"/>
+      <c r="AAT2"/>
+      <c r="AAU2"/>
+      <c r="AAV2"/>
+      <c r="AAW2"/>
+      <c r="AAX2"/>
+      <c r="AAY2"/>
+      <c r="AAZ2"/>
+      <c r="ABA2"/>
+      <c r="ABB2"/>
+      <c r="ABC2"/>
+      <c r="ABD2"/>
+      <c r="ABE2"/>
+      <c r="ABF2"/>
+      <c r="ABG2"/>
+      <c r="ABH2"/>
+      <c r="ABI2"/>
+      <c r="ABJ2"/>
+      <c r="ABK2"/>
+      <c r="ABL2"/>
+      <c r="ABM2"/>
+      <c r="ABN2"/>
+      <c r="ABO2"/>
+      <c r="ABP2"/>
+      <c r="ABQ2"/>
+      <c r="ABR2"/>
+      <c r="ABS2"/>
+      <c r="ABT2"/>
+      <c r="ABU2"/>
+      <c r="ABV2"/>
+      <c r="ABW2"/>
+      <c r="ABX2"/>
+      <c r="ABY2"/>
+      <c r="ABZ2"/>
+      <c r="ACA2"/>
+      <c r="ACB2"/>
+      <c r="ACC2"/>
+      <c r="ACD2"/>
+      <c r="ACE2"/>
+      <c r="ACF2"/>
+      <c r="ACG2"/>
+      <c r="ACH2"/>
+      <c r="ACI2"/>
+      <c r="ACJ2"/>
+      <c r="ACK2"/>
+      <c r="ACL2"/>
+      <c r="ACM2"/>
+      <c r="ACN2"/>
+      <c r="ACO2"/>
+      <c r="ACP2"/>
+      <c r="ACQ2"/>
+      <c r="ACR2"/>
+      <c r="ACS2"/>
+      <c r="ACT2"/>
+      <c r="ACU2"/>
+      <c r="ACV2"/>
+      <c r="ACW2"/>
+      <c r="ACX2"/>
+      <c r="ACY2"/>
+      <c r="ACZ2"/>
+      <c r="ADA2"/>
+      <c r="ADB2"/>
+      <c r="ADC2"/>
+      <c r="ADD2"/>
+      <c r="ADE2"/>
+      <c r="ADF2"/>
+      <c r="ADG2"/>
+      <c r="ADH2"/>
+      <c r="ADI2"/>
+      <c r="ADJ2"/>
+      <c r="ADK2"/>
+      <c r="ADL2"/>
+      <c r="ADM2"/>
+      <c r="ADN2"/>
+      <c r="ADO2"/>
+      <c r="ADP2"/>
+      <c r="ADQ2"/>
+      <c r="ADR2"/>
+      <c r="ADS2"/>
+      <c r="ADT2"/>
+      <c r="ADU2"/>
+      <c r="ADV2"/>
+      <c r="ADW2"/>
+      <c r="ADX2"/>
+      <c r="ADY2"/>
+      <c r="ADZ2"/>
+      <c r="AEA2"/>
+      <c r="AEB2"/>
+      <c r="AEC2"/>
+      <c r="AED2"/>
+      <c r="AEE2"/>
+      <c r="AEF2"/>
+      <c r="AEG2"/>
+      <c r="AEH2"/>
+      <c r="AEI2"/>
+      <c r="AEJ2"/>
+      <c r="AEK2"/>
+      <c r="AEL2"/>
+      <c r="AEM2"/>
+      <c r="AEN2"/>
+      <c r="AEO2"/>
+      <c r="AEP2"/>
+      <c r="AEQ2"/>
+      <c r="AER2"/>
+      <c r="AES2"/>
+      <c r="AET2"/>
+      <c r="AEU2"/>
+      <c r="AEV2"/>
+      <c r="AEW2"/>
+      <c r="AEX2"/>
+      <c r="AEY2"/>
+      <c r="AEZ2"/>
+      <c r="AFA2"/>
+      <c r="AFB2"/>
+      <c r="AFC2"/>
+      <c r="AFD2"/>
+      <c r="AFE2"/>
+      <c r="AFF2"/>
+      <c r="AFG2"/>
+      <c r="AFH2"/>
+      <c r="AFI2"/>
+      <c r="AFJ2"/>
+      <c r="AFK2"/>
+      <c r="AFL2"/>
+      <c r="AFM2"/>
+      <c r="AFN2"/>
+      <c r="AFO2"/>
+      <c r="AFP2"/>
+      <c r="AFQ2"/>
+      <c r="AFR2"/>
+      <c r="AFS2"/>
+      <c r="AFT2"/>
+      <c r="AFU2"/>
+      <c r="AFV2"/>
+      <c r="AFW2"/>
+      <c r="AFX2"/>
+      <c r="AFY2"/>
+      <c r="AFZ2"/>
+      <c r="AGA2"/>
+      <c r="AGB2"/>
+      <c r="AGC2"/>
+      <c r="AGD2"/>
+      <c r="AGE2"/>
+      <c r="AGF2"/>
+      <c r="AGG2"/>
+      <c r="AGH2"/>
+      <c r="AGI2"/>
+      <c r="AGJ2"/>
+      <c r="AGK2"/>
+      <c r="AGL2"/>
+      <c r="AGM2"/>
+      <c r="AGN2"/>
+      <c r="AGO2"/>
+      <c r="AGP2"/>
+      <c r="AGQ2"/>
+      <c r="AGR2"/>
+      <c r="AGS2"/>
+      <c r="AGT2"/>
+      <c r="AGU2"/>
+      <c r="AGV2"/>
+      <c r="AGW2"/>
+      <c r="AGX2"/>
+      <c r="AGY2"/>
+      <c r="AGZ2"/>
+      <c r="AHA2"/>
+      <c r="AHB2"/>
+      <c r="AHC2"/>
+      <c r="AHD2"/>
+      <c r="AHE2"/>
+      <c r="AHF2"/>
+      <c r="AHG2"/>
+      <c r="AHH2"/>
+      <c r="AHI2"/>
+      <c r="AHJ2"/>
+      <c r="AHK2"/>
+      <c r="AHL2"/>
+      <c r="AHM2"/>
+      <c r="AHN2"/>
+      <c r="AHO2"/>
+      <c r="AHP2"/>
+      <c r="AHQ2"/>
+      <c r="AHR2"/>
+      <c r="AHS2"/>
+      <c r="AHT2"/>
+      <c r="AHU2"/>
+      <c r="AHV2"/>
+      <c r="AHW2"/>
+      <c r="AHX2"/>
+      <c r="AHY2"/>
+      <c r="AHZ2"/>
+      <c r="AIA2"/>
+      <c r="AIB2"/>
+      <c r="AIC2"/>
+      <c r="AID2"/>
+      <c r="AIE2"/>
+      <c r="AIF2"/>
+      <c r="AIG2"/>
+      <c r="AIH2"/>
+      <c r="AII2"/>
+      <c r="AIJ2"/>
+      <c r="AIK2"/>
+      <c r="AIL2"/>
+      <c r="AIM2"/>
+      <c r="AIN2"/>
+      <c r="AIO2"/>
+      <c r="AIP2"/>
+      <c r="AIQ2"/>
+      <c r="AIR2"/>
+      <c r="AIS2"/>
+      <c r="AIT2"/>
+      <c r="AIU2"/>
+      <c r="AIV2"/>
+      <c r="AIW2"/>
+      <c r="AIX2"/>
+      <c r="AIY2"/>
+      <c r="AIZ2"/>
+      <c r="AJA2"/>
+      <c r="AJB2"/>
+      <c r="AJC2"/>
+      <c r="AJD2"/>
+      <c r="AJE2"/>
+      <c r="AJF2"/>
+      <c r="AJG2"/>
+      <c r="AJH2"/>
+      <c r="AJI2"/>
+      <c r="AJJ2"/>
+      <c r="AJK2"/>
+      <c r="AJL2"/>
+      <c r="AJM2"/>
+      <c r="AJN2"/>
+      <c r="AJO2"/>
+      <c r="AJP2"/>
+      <c r="AJQ2"/>
+      <c r="AJR2"/>
+      <c r="AJS2"/>
+      <c r="AJT2"/>
+      <c r="AJU2"/>
+      <c r="AJV2"/>
+      <c r="AJW2"/>
+      <c r="AJX2"/>
+      <c r="AJY2"/>
+      <c r="AJZ2"/>
+      <c r="AKA2"/>
+      <c r="AKB2"/>
+      <c r="AKC2"/>
+      <c r="AKD2"/>
+      <c r="AKE2"/>
+      <c r="AKF2"/>
+      <c r="AKG2"/>
+      <c r="AKH2"/>
+      <c r="AKI2"/>
+      <c r="AKJ2"/>
+      <c r="AKK2"/>
+      <c r="AKL2"/>
+      <c r="AKM2"/>
+      <c r="AKN2"/>
+      <c r="AKO2"/>
+      <c r="AKP2"/>
+      <c r="AKQ2"/>
+      <c r="AKR2"/>
+      <c r="AKS2"/>
+      <c r="AKT2"/>
+      <c r="AKU2"/>
+      <c r="AKV2"/>
+      <c r="AKW2"/>
+      <c r="AKX2"/>
+      <c r="AKY2"/>
+      <c r="AKZ2"/>
+      <c r="ALA2"/>
+      <c r="ALB2"/>
+      <c r="ALC2"/>
+      <c r="ALD2"/>
+      <c r="ALE2"/>
+      <c r="ALF2"/>
+      <c r="ALG2"/>
+      <c r="ALH2"/>
+      <c r="ALI2"/>
+      <c r="ALJ2"/>
+      <c r="ALK2"/>
+      <c r="ALL2"/>
+      <c r="ALM2"/>
+      <c r="ALN2"/>
+      <c r="ALO2"/>
+      <c r="ALP2"/>
+      <c r="ALQ2"/>
+      <c r="ALR2"/>
+      <c r="ALS2"/>
+      <c r="ALT2"/>
+      <c r="ALU2"/>
+      <c r="ALV2"/>
+      <c r="ALW2"/>
+      <c r="ALX2"/>
+      <c r="ALY2"/>
+      <c r="ALZ2"/>
+      <c r="AMA2"/>
+      <c r="AMB2"/>
+      <c r="AMC2"/>
+      <c r="AMD2"/>
+      <c r="AME2"/>
+      <c r="AMF2"/>
+      <c r="AMG2"/>
+      <c r="AMH2"/>
+    </row>
+    <row r="3" spans="1:1022" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1022" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>13</v>
+    <row r="5" spans="1:1022" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1022" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B7" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B8" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B10" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B11" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B12" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B13" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B14" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B15" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:1022" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B16" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
         <v>85</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
         <v>87</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C56" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C57" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C58" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C66" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C67" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D71" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D72" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D73" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C74" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D74" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C75" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D75" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D76" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D79" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C80" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D80" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C81" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D81" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C82" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D82" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C83" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D83" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C84" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D84" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>178</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="C85" t="s">
-        <v>19</v>
-      </c>
-      <c r="D85" t="s">
-        <v>179</v>
-      </c>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B86" s="6"/>
@@ -2887,12 +3907,9 @@
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" s="6"/>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B176" s="6"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" sqref="B4:B176 C6:C85" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showErrorMessage="1" sqref="C5:C84 B4:B175" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2921,16 +3938,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>